<commit_message>
Add spreadsheet URL to config for RPA
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29f27606214cd687/Documents/UiPath/BOT1(new)/Bot1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\UiPath\Bot1_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{76919E00-8C62-4E5C-AEA5-C98D2790DA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E063FF-649C-43F8-B969-CDD1D7A8BD15}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D999D-89CF-405E-9C19-E41350A3679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{05E979CD-2C89-4B74-8A78-07879031F12A}"/>
   </bookViews>
@@ -33,8 +33,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ASUS</author>
+  </authors>
+  <commentList>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{ED9F0B40-3107-4585-AF08-F87999D14C67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Description:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+List of destination emails to be sent.
+You can enter several in a vertical order</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{C909CCB6-B189-4B56-8581-BE4B3297DB65}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Description:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+List of email owner names to be sent. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -45,26 +104,56 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Penerima Email, gunakan ";" antar variabel, dan gunakan "," untuk Posisi </t>
-  </si>
-  <si>
-    <t>email_Receipt</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>zeerx7@gmail.com,Leader; pausi347@gmail.com,HC Team; rosadirully5@gmail.com,Leader</t>
-  </si>
-  <si>
     <t>New Employe Boarding Annoucement September 2023</t>
+  </si>
+  <si>
+    <t>Email Recipients</t>
+  </si>
+  <si>
+    <t>zeerx7@gmail.com</t>
+  </si>
+  <si>
+    <t>pausi347@gmail.com</t>
+  </si>
+  <si>
+    <t>Leader</t>
+  </si>
+  <si>
+    <t>HC TEam</t>
+  </si>
+  <si>
+    <t>rosadirully5@gmail.com</t>
+  </si>
+  <si>
+    <t>Spreadsheet URL</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/165orIVd662-v-6BYnt8sJLENrY0tvxh3NYk63mj_Tnk/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Email Subject</t>
+  </si>
+  <si>
+    <t>Subject of the email to be sent.</t>
+  </si>
+  <si>
+    <t>Spreadsheet URL containing the Offering Letter Report.</t>
+  </si>
+  <si>
+    <t>the name of the sheet in the spreadsheet.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +169,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -105,14 +216,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -129,9 +243,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +283,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -275,7 +389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,24 +531,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E606130A-4C41-4C34-BD15-EC79FD154BCD}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E606130A-4C41-4C34-BD15-EC79FD154BCD}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99" customWidth="1"/>
     <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -451,24 +565,76 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{3D10A026-1604-466A-BF49-56C90353A610}"/>
+    <hyperlink ref="A9" r:id="rId2" xr:uid="{3EB48A27-7068-4FFB-8E02-51CB9F7AD3DF}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{26816AC9-9173-4BE2-98B4-C8D254AAEF78}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Email Text to config and apply it to RPA
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\UiPath\Bot1_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D999D-89CF-405E-9C19-E41350A3679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5C3DE2-D62A-4FA3-8FDD-4A5D42FA9380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{05E979CD-2C89-4B74-8A78-07879031F12A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>ASUS</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{ED9F0B40-3107-4585-AF08-F87999D14C67}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{ED9F0B40-3107-4585-AF08-F87999D14C67}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{C909CCB6-B189-4B56-8581-BE4B3297DB65}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{C909CCB6-B189-4B56-8581-BE4B3297DB65}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>the name of the sheet in the spreadsheet.</t>
+  </si>
+  <si>
+    <t>Email Text</t>
+  </si>
+  <si>
+    <t>Mohon dapat disiapkan laptop dan email untuk Talents yang akan boarding dengan detail sebagai berikut:</t>
+  </si>
+  <si>
+    <t>Text to be displayed in the body of the email</t>
   </si>
 </sst>
 </file>
@@ -539,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E606130A-4C41-4C34-BD15-EC79FD154BCD}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,74 +574,85 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{3D10A026-1604-466A-BF49-56C90353A610}"/>
-    <hyperlink ref="A9" r:id="rId2" xr:uid="{3EB48A27-7068-4FFB-8E02-51CB9F7AD3DF}"/>
-    <hyperlink ref="A7" r:id="rId3" xr:uid="{26816AC9-9173-4BE2-98B4-C8D254AAEF78}"/>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{3D10A026-1604-466A-BF49-56C90353A610}"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{3EB48A27-7068-4FFB-8E02-51CB9F7AD3DF}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{26816AC9-9173-4BE2-98B4-C8D254AAEF78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId4"/>

</xml_diff>